<commit_message>
Extract DacAuthorisation data from Suivi TRI_TRE file
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSource/Suivi TRI_TRE.xlsx
+++ b/src/main/resources/dataSource/Suivi TRI_TRE.xlsx
@@ -1053,6 +1053,30 @@
   <si>
     <t>sieAu</t>
   </si>
+  <si>
+    <t>N° Aut TRI</t>
+  </si>
+  <si>
+    <t>DuTRI</t>
+  </si>
+  <si>
+    <t>AuTRI</t>
+  </si>
+  <si>
+    <t>N° Aut TRE</t>
+  </si>
+  <si>
+    <t>DuTRE</t>
+  </si>
+  <si>
+    <t>AuTRE</t>
+  </si>
+  <si>
+    <t>DuFI_ATPL</t>
+  </si>
+  <si>
+    <t>AuFI_ATPL</t>
+  </si>
 </sst>
 </file>
 
@@ -1061,7 +1085,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1073,6 +1097,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <color theme="1"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Segoe UI"/>
+      <color rgb="FF000000"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1113,7 +1143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
       <alignment vertical="bottom"/>
@@ -1122,6 +1152,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="16" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1428,13 +1461,21 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1460,28 +1501,28 @@
         <v>343</v>
       </c>
       <c r="H1" t="s">
-        <v>16</v>
+        <v>346</v>
       </c>
       <c r="I1" t="s">
-        <v>17</v>
+        <v>347</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>348</v>
       </c>
       <c r="K1" t="s">
-        <v>16</v>
+        <v>349</v>
       </c>
       <c r="L1" t="s">
-        <v>17</v>
+        <v>350</v>
       </c>
       <c r="M1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" t="s">
-        <v>17</v>
+        <v>351</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>352</v>
       </c>
       <c r="O1" t="s">
-        <v>18</v>
+        <v>353</v>
       </c>
       <c r="P1" t="s">
         <v>344</v>

</xml_diff>

<commit_message>
Extract InstructorObservation data from Suivi TRI_TRE file
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSource/Suivi TRI_TRE.xlsx
+++ b/src/main/resources/dataSource/Suivi TRI_TRE.xlsx
@@ -1076,6 +1076,24 @@
   </si>
   <si>
     <t>AuFI_ATPL</t>
+  </si>
+  <si>
+    <t>SIEHabilitation</t>
+  </si>
+  <si>
+    <t>DteHabilitation</t>
+  </si>
+  <si>
+    <t>TRESimuPlaceDroite</t>
+  </si>
+  <si>
+    <t>DteSimuPlaceDroite</t>
+  </si>
+  <si>
+    <t>DteDG</t>
+  </si>
+  <si>
+    <t>SIEDG</t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
       <alignment vertical="bottom"/>
@@ -1156,6 +1174,9 @@
     </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="14" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1460,8 +1481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
-      <selection activeCell="I4" activeCellId="0" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="I73">
+      <selection activeCell="T81" activeCellId="0" sqref="T81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1476,6 +1497,10 @@
     <col min="13" max="13" width="11.42578125" customWidth="1"/>
     <col min="14" max="14" width="11.42578125" customWidth="1"/>
     <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="19" max="19" width="4.5703125" customWidth="1"/>
+    <col min="20" max="20" width="14.85546875" customWidth="1"/>
+    <col min="21" max="21" width="20.5703125" customWidth="1"/>
+    <col min="22" max="22" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1537,22 +1562,22 @@
         <v>20</v>
       </c>
       <c r="T1" t="s">
-        <v>19</v>
+        <v>355</v>
       </c>
       <c r="U1" t="s">
-        <v>4</v>
+        <v>354</v>
       </c>
       <c r="V1" t="s">
-        <v>21</v>
+        <v>357</v>
       </c>
       <c r="W1" t="s">
-        <v>22</v>
+        <v>356</v>
       </c>
       <c r="X1" t="s">
-        <v>19</v>
+        <v>358</v>
       </c>
       <c r="Y1" t="s">
-        <v>4</v>
+        <v>359</v>
       </c>
       <c r="Z1" t="s">
         <v>23</v>
@@ -5179,7 +5204,7 @@
       <c r="Q81" t="s">
         <v>28</v>
       </c>
-      <c r="T81" s="3">
+      <c r="T81" s="5">
         <v>45389</v>
       </c>
       <c r="U81" t="s">

</xml_diff>

<commit_message>
Extract InstructorSimuPlaceDroite data from Suivi TRI_TRE file
</commit_message>
<xml_diff>
--- a/src/main/resources/dataSource/Suivi TRI_TRE.xlsx
+++ b/src/main/resources/dataSource/Suivi TRI_TRE.xlsx
@@ -1481,8 +1481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="I73">
-      <selection activeCell="T81" activeCellId="0" sqref="T81"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="P1">
+      <selection activeCell="Y21" activeCellId="0" sqref="Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1501,6 +1501,8 @@
     <col min="20" max="20" width="14.85546875" customWidth="1"/>
     <col min="21" max="21" width="20.5703125" customWidth="1"/>
     <col min="22" max="22" width="16.140625" customWidth="1"/>
+    <col min="24" max="24" width="16" customWidth="1"/>
+    <col min="25" max="25" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2571,7 +2573,7 @@
         <v>44555</v>
       </c>
       <c r="Y21" t="s">
-        <v>108</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22">

</xml_diff>